<commit_message>
try catch and exception handling
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Betty\Desktop\RpaProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANUL3\rapa\Proiect\RpaProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7117232A-46B6-441A-AB09-A484C90F92B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6036"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Email</t>
   </si>
@@ -51,9 +52,6 @@
   </si>
   <si>
     <t>IT-Software</t>
-  </si>
-  <si>
-    <t>bucuresti</t>
   </si>
   <si>
     <t>Ploiesti</t>
@@ -77,7 +75,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -399,11 +397,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -433,10 +431,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -446,9 +444,6 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
@@ -456,10 +451,10 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -476,16 +471,16 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
implemented kill process as exception handling
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANUL3\rapa\Proiect\RpaProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7117232A-46B6-441A-AB09-A484C90F92B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD24B27-C3F9-42E8-9D87-2DC05EDB28EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Email</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>"part-time"</t>
+  </si>
+  <si>
+    <t>IT-Softwardfghje</t>
   </si>
 </sst>
 </file>
@@ -401,7 +404,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,8 +447,11 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
changed some activity names
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -71,7 +71,7 @@
     <t>0 - 1 an experienta,1 - 5 ani experienta</t>
   </si>
   <si>
-    <t>part-time,practica</t>
+    <t>full-time</t>
   </si>
 </sst>
 </file>
@@ -403,7 +403,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
improved job application method
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Betty\Desktop\RpaProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANUL3\rapa\Proiect\RpaProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAFA477-82A6-464C-A862-963035C17C6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,16 +69,16 @@
     <t>bucuresti</t>
   </si>
   <si>
-    <t>0 - 1 an experienta,1 - 5 ani experienta</t>
-  </si>
-  <si>
     <t>full-time</t>
+  </si>
+  <si>
+    <t>0 - 1 an experienta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -399,11 +400,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,10 +457,10 @@
         <v>13</v>
       </c>
       <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -484,8 +485,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
refactored the job application method
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANUL3\rapa\Proiect\RpaProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Betty\Desktop\RpaProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAFA477-82A6-464C-A862-963035C17C6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,16 +68,16 @@
     <t>bucuresti</t>
   </si>
   <si>
+    <t>0 - 1 an experienta</t>
+  </si>
+  <si>
     <t>full-time</t>
-  </si>
-  <si>
-    <t>0 - 1 an experienta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -400,11 +399,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,10 +456,10 @@
         <v>13</v>
       </c>
       <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
         <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -485,8 +484,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
tested and refactored job application method
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>Email</t>
   </si>
@@ -53,15 +53,9 @@
     <t>IT-Software</t>
   </si>
   <si>
-    <t>Ploiesti</t>
-  </si>
-  <si>
     <t>Experience</t>
   </si>
   <si>
-    <t>""</t>
-  </si>
-  <si>
     <t>Job Type</t>
   </si>
   <si>
@@ -72,6 +66,54 @@
   </si>
   <si>
     <t>full-time</t>
+  </si>
+  <si>
+    <t>profesor</t>
+  </si>
+  <si>
+    <t>Educatie-Training</t>
+  </si>
+  <si>
+    <t>Bucuresti</t>
+  </si>
+  <si>
+    <t>Student--Absolvent</t>
+  </si>
+  <si>
+    <t>part-time</t>
+  </si>
+  <si>
+    <t>inginer</t>
+  </si>
+  <si>
+    <t>Timisoara</t>
+  </si>
+  <si>
+    <t>peste 5 ani experienta,Manager</t>
+  </si>
+  <si>
+    <t>Inginerie</t>
+  </si>
+  <si>
+    <t>secretar</t>
+  </si>
+  <si>
+    <t>Secretariat-Administrativ</t>
+  </si>
+  <si>
+    <t>0 - 1 an experienta,1 - 5 ani experienta</t>
+  </si>
+  <si>
+    <t>full-time,practica</t>
+  </si>
+  <si>
+    <t>legal</t>
+  </si>
+  <si>
+    <t>Juridic</t>
+  </si>
+  <si>
+    <t>1 - 5 ani experienta</t>
   </si>
 </sst>
 </file>
@@ -400,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -433,10 +475,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -447,19 +489,19 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -470,22 +512,97 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="E6" t="s">
         <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A6" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId4"/>
+    <hyperlink ref="A3" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added exception handlers, implemented terminate workflows
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Betty\Desktop\RpaProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANUL3\rapa\Proiect\RpaProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B88299-E06D-4B75-8783-801B362F2906}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>Email</t>
   </si>
@@ -114,12 +115,15 @@
   </si>
   <si>
     <t>1 - 5 ani experienta</t>
+  </si>
+  <si>
+    <t>0 - 1 fdghnta,1 - 5 an</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -441,11 +445,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,7 +502,7 @@
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
         <v>26</v>
@@ -512,19 +516,19 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -535,16 +539,16 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
         <v>13</v>
@@ -558,19 +562,19 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -581,28 +585,52 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>8</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>11</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" t="s">
         <v>12</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1"/>
-    <hyperlink ref="A4" r:id="rId2"/>
-    <hyperlink ref="A5" r:id="rId3"/>
-    <hyperlink ref="A2" r:id="rId4"/>
-    <hyperlink ref="A3" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A2" r:id="rId6" xr:uid="{6EE857A7-175E-42C9-9605-BCA07EFA6AD3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>